<commit_message>
Entity 'UnitOfMeasure' was fixed.
</commit_message>
<xml_diff>
--- a/src/main/resources/Basic_data.xlsx
+++ b/src/main/resources/Basic_data.xlsx
@@ -5,23 +5,24 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java practice\api\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java practice\naakcii_api2\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Basic_chains" sheetId="11" r:id="rId1"/>
-    <sheet name="Basic_categories " sheetId="12" r:id="rId2"/>
-    <sheet name="Basic_action_types" sheetId="13" r:id="rId3"/>
+    <sheet name="Basic_categories" sheetId="12" r:id="rId2"/>
+    <sheet name="Basic_subcategories" sheetId="14" r:id="rId3"/>
+    <sheet name="Basic_action_types" sheetId="13" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="111">
   <si>
     <t>Торговая сеть</t>
   </si>
@@ -120,6 +121,240 @@
   </si>
   <si>
     <t>1+1</t>
+  </si>
+  <si>
+    <t>Хлебобулочные изделия</t>
+  </si>
+  <si>
+    <t>Сдобные изделия</t>
+  </si>
+  <si>
+    <t>Хлеб, батон</t>
+  </si>
+  <si>
+    <t>Хлебцы</t>
+  </si>
+  <si>
+    <t>Овощи и фрукты</t>
+  </si>
+  <si>
+    <t>Грибы</t>
+  </si>
+  <si>
+    <t>Овощи</t>
+  </si>
+  <si>
+    <t>Фрукты</t>
+  </si>
+  <si>
+    <t>Ягоды</t>
+  </si>
+  <si>
+    <t>Молочные продукты, яйца</t>
+  </si>
+  <si>
+    <t>Мясо и колбасные изделия</t>
+  </si>
+  <si>
+    <t>Напитки, кофе, чай, соки</t>
+  </si>
+  <si>
+    <t>Бакалея</t>
+  </si>
+  <si>
+    <t>Рыба и морепродукты</t>
+  </si>
+  <si>
+    <t>Сладости</t>
+  </si>
+  <si>
+    <t>Замороженные продукты</t>
+  </si>
+  <si>
+    <t>Детское питание</t>
+  </si>
+  <si>
+    <t>Собственное производство</t>
+  </si>
+  <si>
+    <t>Кисломолочные изделия</t>
+  </si>
+  <si>
+    <t>Масло</t>
+  </si>
+  <si>
+    <t>Молоко</t>
+  </si>
+  <si>
+    <t>Мороженое</t>
+  </si>
+  <si>
+    <t>Сметана</t>
+  </si>
+  <si>
+    <t>Сыр</t>
+  </si>
+  <si>
+    <t>Творожные продукты</t>
+  </si>
+  <si>
+    <t>Яйцо</t>
+  </si>
+  <si>
+    <t>Синоним</t>
+  </si>
+  <si>
+    <t>bel-market</t>
+  </si>
+  <si>
+    <t>prostore</t>
+  </si>
+  <si>
+    <t>rublevski</t>
+  </si>
+  <si>
+    <t>sosedi</t>
+  </si>
+  <si>
+    <t>vitalur</t>
+  </si>
+  <si>
+    <t>evroopt</t>
+  </si>
+  <si>
+    <t>korona</t>
+  </si>
+  <si>
+    <t>almi</t>
+  </si>
+  <si>
+    <t>Говядина</t>
+  </si>
+  <si>
+    <t>Колбасные изделия</t>
+  </si>
+  <si>
+    <t>Копчености</t>
+  </si>
+  <si>
+    <t>Птица</t>
+  </si>
+  <si>
+    <t>Свинина</t>
+  </si>
+  <si>
+    <t>Другие виды мяса</t>
+  </si>
+  <si>
+    <t>Вода</t>
+  </si>
+  <si>
+    <t>Кофе и заменители</t>
+  </si>
+  <si>
+    <t>Напитки</t>
+  </si>
+  <si>
+    <t>Соки</t>
+  </si>
+  <si>
+    <t>Чай</t>
+  </si>
+  <si>
+    <t>Консервированная продукция</t>
+  </si>
+  <si>
+    <t>Крупы, бобовые</t>
+  </si>
+  <si>
+    <t>Макароны</t>
+  </si>
+  <si>
+    <t>Масло растительное, уксус</t>
+  </si>
+  <si>
+    <t>Мука</t>
+  </si>
+  <si>
+    <t>Продукты быстрого приготовления</t>
+  </si>
+  <si>
+    <t>Снеки</t>
+  </si>
+  <si>
+    <t>Соусы</t>
+  </si>
+  <si>
+    <t>Специи и кондитерские добавки</t>
+  </si>
+  <si>
+    <t>Сухие завтраки</t>
+  </si>
+  <si>
+    <t>Сухофрукты</t>
+  </si>
+  <si>
+    <t>Закуски из рыбы и морепродуктов</t>
+  </si>
+  <si>
+    <t>Икра</t>
+  </si>
+  <si>
+    <t>Морепродукты</t>
+  </si>
+  <si>
+    <t>Рыба</t>
+  </si>
+  <si>
+    <t>Бисквиты и печенье</t>
+  </si>
+  <si>
+    <t>Другие сладости</t>
+  </si>
+  <si>
+    <t>Торты, пирожные</t>
+  </si>
+  <si>
+    <t>Шоколад и конфеты</t>
+  </si>
+  <si>
+    <t>Полуфабрикаты</t>
+  </si>
+  <si>
+    <t>Ягоды, фрукты</t>
+  </si>
+  <si>
+    <t>Каши</t>
+  </si>
+  <si>
+    <t>Консервы</t>
+  </si>
+  <si>
+    <t>Пюре</t>
+  </si>
+  <si>
+    <t>Сухие смеси</t>
+  </si>
+  <si>
+    <t>Вторые блюда</t>
+  </si>
+  <si>
+    <t>Десерты</t>
+  </si>
+  <si>
+    <t>Салаты и закуски</t>
+  </si>
+  <si>
+    <t>Супы</t>
+  </si>
+  <si>
+    <t>discount</t>
+  </si>
+  <si>
+    <t>good_price</t>
+  </si>
+  <si>
+    <t>one_plus_one</t>
   </si>
 </sst>
 </file>
@@ -141,14 +376,14 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,12 +393,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -187,44 +416,52 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -505,127 +742,154 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="24.875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="11.875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="18" style="9" customWidth="1"/>
+    <col min="1" max="4" width="15.625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="15.625" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="C7" s="4"/>
+      <c r="D7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="C8" s="4"/>
+      <c r="D8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>23</v>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -636,53 +900,1022 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" style="5" customWidth="1"/>
-    <col min="2" max="2" width="24.25" style="5" customWidth="1"/>
-    <col min="3" max="5" width="18" style="5" customWidth="1"/>
+    <col min="1" max="1" width="25.625" style="14" customWidth="1"/>
+    <col min="2" max="4" width="15.625" style="14" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="13">
+        <v>100</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="15">
+        <v>200</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="15">
+        <v>300</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="15">
+        <v>400</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="15">
+        <v>700</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="15">
+        <v>500</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="15">
+        <v>600</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="15">
+        <v>10000</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="15">
+        <v>900</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="15">
+        <v>800</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="15">
+        <v>1100</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D60"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="25.625" style="9" customWidth="1"/>
+    <col min="3" max="4" width="15.625" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="11" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>26</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="16">
+        <v>400</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="16">
+        <v>600</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="16">
+        <v>800</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="16">
+        <v>100</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="16">
+        <v>500</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="16">
+        <v>200</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="16">
+        <v>300</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="16">
+        <v>700</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="16">
+        <v>200</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="16">
+        <v>300</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="16">
+        <v>100</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="16">
+        <v>200</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="16">
+        <v>400</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="16">
+        <v>300</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="16">
+        <v>100</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="18">
+        <v>400</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="18">
+        <v>300</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="18">
+        <v>200</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="18">
+        <v>600</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="18">
+        <v>500</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="18">
+        <v>100</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="18">
+        <v>500</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="18">
+        <v>300</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="18">
+        <v>100</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="18">
+        <v>200</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="18">
+        <v>400</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="18">
+        <v>700</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="18">
+        <v>10000</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="18">
+        <v>11000</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="18">
+        <v>800</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="18">
+        <v>900</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="18">
+        <v>500</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="18">
+        <v>200</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="18">
+        <v>400</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="18">
+        <v>300</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="18">
+        <v>600</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="18">
+        <v>100</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="18">
+        <v>200</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="18">
+        <v>100</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="18">
+        <v>300</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" s="18">
+        <v>400</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="18">
+        <v>300</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="18">
+        <v>100</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" s="18">
+        <v>200</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" s="18">
+        <v>400</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C48" s="18">
+        <v>200</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" s="18">
+        <v>300</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" s="18">
+        <v>400</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" s="18">
+        <v>100</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C52" s="18">
+        <v>400</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C53" s="18">
+        <v>100</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C54" s="18">
+        <v>300</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C55" s="18">
+        <v>200</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C56" s="18">
+        <v>500</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C57" s="18">
+        <v>400</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C58" s="18">
+        <v>100</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C59" s="18">
+        <v>200</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C60" s="18">
+        <v>300</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -690,44 +1923,58 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18" style="5" customWidth="1"/>
-    <col min="3" max="4" width="18" customWidth="1"/>
+    <col min="1" max="2" width="18" style="14" customWidth="1"/>
+    <col min="3" max="4" width="18" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="C1" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="C2" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="C3" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>32</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Multi sheet importer (parser) v.0.91.
</commit_message>
<xml_diff>
--- a/src/main/resources/Basic_data.xlsx
+++ b/src/main/resources/Basic_data.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Basic_chains" sheetId="11" r:id="rId1"/>
     <sheet name="Basic_categories" sheetId="12" r:id="rId2"/>
     <sheet name="Basic_subcategories" sheetId="14" r:id="rId3"/>
-    <sheet name="Basic_action_types" sheetId="13" r:id="rId4"/>
+    <sheet name="Basic_chain_product_types" sheetId="13" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -902,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,7 +1020,7 @@
         <v>47</v>
       </c>
       <c r="B10" s="15">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>23</v>
@@ -1927,8 +1927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1969,6 +1969,7 @@
       <c r="A4" s="14" t="s">
         <v>32</v>
       </c>
+      <c r="B4" s="4"/>
       <c r="C4" s="9" t="s">
         <v>110</v>
       </c>

</xml_diff>